<commit_message>
set color of C strategy to black in all graphs
</commit_message>
<xml_diff>
--- a/results/results_generated.xlsx
+++ b/results/results_generated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groschri\Seafile\My Library\uni\long-term-fairness\results\output_generated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groschri\Seafile\My Library\uni\long-term-fairness\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -251,6 +251,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -347,7 +348,13 @@
             <c:symbol val="diamond"/>
             <c:size val="5"/>
             <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
               <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
@@ -1202,11 +1209,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1278292384"/>
-        <c:axId val="-1278300544"/>
+        <c:axId val="1297132912"/>
+        <c:axId val="1297124752"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-1278300544"/>
+        <c:axId val="1297124752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,12 +1243,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1278292384"/>
+        <c:crossAx val="1297132912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1278292384"/>
+        <c:axId val="1297132912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1278300544"/>
+        <c:crossAx val="1297124752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1347,7 +1354,13 @@
             <c:symbol val="diamond"/>
             <c:size val="5"/>
             <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
               <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
@@ -2202,11 +2215,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1278300000"/>
-        <c:axId val="-1278301632"/>
+        <c:axId val="1297127472"/>
+        <c:axId val="1297122576"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-1278301632"/>
+        <c:axId val="1297122576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2236,12 +2249,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1278300000"/>
+        <c:crossAx val="1297127472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1278300000"/>
+        <c:axId val="1297127472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2274,7 +2287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1278301632"/>
+        <c:crossAx val="1297122576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2634,11 +2647,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1278297824"/>
-        <c:axId val="-1278295104"/>
+        <c:axId val="1297121488"/>
+        <c:axId val="1297131280"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-1278295104"/>
+        <c:axId val="1297131280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2668,12 +2681,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1278297824"/>
+        <c:crossAx val="1297121488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1278297824"/>
+        <c:axId val="1297121488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2705,7 +2718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1278295104"/>
+        <c:crossAx val="1297131280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3110,7 +3123,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>